<commit_message>
Add inventories for industrial heat pump
</commit_message>
<xml_diff>
--- a/premise/data/utils/import/classifications.xlsx
+++ b/premise/data/utils/import/classifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/utils/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953C614F-BBB1-A742-820C-2994CACEB4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548C4DCB-B0AD-2141-A7D6-F1A10E54B44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40160" yWindow="-680" windowWidth="29840" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12300" uniqueCount="3434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12312" uniqueCount="3440">
   <si>
     <t>name</t>
   </si>
@@ -10338,6 +10338,24 @@
   </si>
   <si>
     <t>transport, freight, lorry, gasoline, 3.5 metric ton</t>
+  </si>
+  <si>
+    <t>heat pump production, industrial, water-water, 100 kW</t>
+  </si>
+  <si>
+    <t>heat pump, water-water, 100kW</t>
+  </si>
+  <si>
+    <t>steam heat production, water-water heat pump, industrial, 100kW</t>
+  </si>
+  <si>
+    <t>steam heat, water-water heat pump, industrial, 100kW</t>
+  </si>
+  <si>
+    <t>heat production, water-water heat pump, industrial, 100kW</t>
+  </si>
+  <si>
+    <t>heat, water-water heat pump, industrial, 100kW</t>
   </si>
 </sst>
 </file>
@@ -10705,10 +10723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3075"/>
+  <dimension ref="A1:D3078"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2601" workbookViewId="0">
-      <selection activeCell="C2636" sqref="C2636"/>
+    <sheetView tabSelected="1" topLeftCell="A3034" workbookViewId="0">
+      <selection activeCell="C3077" sqref="C3077"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53769,6 +53787,48 @@
         <v>2741</v>
       </c>
     </row>
+    <row r="3076" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3076" t="s">
+        <v>3434</v>
+      </c>
+      <c r="B3076" t="s">
+        <v>3435</v>
+      </c>
+      <c r="C3076" t="s">
+        <v>2649</v>
+      </c>
+      <c r="D3076" t="s">
+        <v>2691</v>
+      </c>
+    </row>
+    <row r="3077" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3077" t="s">
+        <v>3436</v>
+      </c>
+      <c r="B3077" t="s">
+        <v>3437</v>
+      </c>
+      <c r="C3077" t="s">
+        <v>2647</v>
+      </c>
+      <c r="D3077" t="s">
+        <v>2683</v>
+      </c>
+    </row>
+    <row r="3078" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3078" t="s">
+        <v>3438</v>
+      </c>
+      <c r="B3078" t="s">
+        <v>3439</v>
+      </c>
+      <c r="C3078" t="s">
+        <v>2647</v>
+      </c>
+      <c r="D3078" t="s">
+        <v>2683</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D3075" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D3075">

</xml_diff>

<commit_message>
Improve Pathways data package export
</commit_message>
<xml_diff>
--- a/premise/data/utils/import/classifications.xlsx
+++ b/premise/data/utils/import/classifications.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/utils/import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/utils/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC3790E-1F2D-7B42-AF07-4F0F0C6FD8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A40AB3-8371-B340-9262-32154576A634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="33940" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$3142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$3155</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12614" uniqueCount="3553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12616" uniqueCount="3553">
   <si>
     <t>name</t>
   </si>
@@ -11064,8 +11064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3138" workbookViewId="0">
-      <selection activeCell="B3161" sqref="B3161"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54981,6 +54981,12 @@
       <c r="B3137" t="s">
         <v>3536</v>
       </c>
+      <c r="C3137" t="s">
+        <v>2656</v>
+      </c>
+      <c r="D3137" t="s">
+        <v>2741</v>
+      </c>
     </row>
     <row r="3138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3138" t="s">
@@ -55229,7 +55235,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D3142" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D3155" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>